<commit_message>
updated pie-chart to include numbers, fixed #81
</commit_message>
<xml_diff>
--- a/timing-pie-chart/pie-chart-overview.xlsx
+++ b/timing-pie-chart/pie-chart-overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gernotstarke/projects/isaqb/pie-chart/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gernotstarke/projects/isaqb/curriculum-foundation/timing-pie-chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37863F1A-C6F7-7D42-ADFE-8B56575DA3D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EEB146-0993-1A44-91F4-651C56D206BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="2640" windowWidth="20700" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="2640" windowWidth="20700" windowHeight="15360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EN-Graphic" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28487233288398001"/>
+          <c:y val="9.3791529332182016E-2"/>
+          <c:w val="0.45586669437757921"/>
+          <c:h val="0.86077659921177563"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -223,7 +233,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -244,7 +254,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -265,7 +275,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -286,7 +296,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -307,7 +317,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -328,7 +338,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -348,7 +358,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -538,7 +548,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -559,7 +569,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -580,7 +590,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -601,7 +611,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -622,7 +632,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -643,7 +653,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -663,7 +673,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -1168,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1231,6 +1241,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1239,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1327,7 +1338,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new timing (see issue #99)
https://github.com/isaqb-org/curriculum-foundation/issues/99
</commit_message>
<xml_diff>
--- a/timing-pie-chart/pie-chart-overview.xlsx
+++ b/timing-pie-chart/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gernotstarke/projects/isaqb/curriculum-foundation/timing-pie-chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EEB146-0993-1A44-91F4-651C56D206BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78513A5B-7F3C-7349-AC2B-E1014585AD85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="2640" windowWidth="20700" windowHeight="15360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="1180" windowWidth="20700" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EN-Graphic" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,10 @@
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>450</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>120</c:v>
@@ -716,10 +716,10 @@
                   <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>450</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>120</c:v>
@@ -1178,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B2">
         <f>Times!D3</f>
-        <v>450</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="B3">
         <f>Times!D4</f>
-        <v>300</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1236,7 +1236,7 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6">
         <f>SUM(B1:B5)</f>
-        <v>1080</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="B2">
         <f>Times!D3</f>
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="B3">
         <f>Times!D4</f>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1323,7 +1323,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6">
         <f>SUM(B1:B5)</f>
-        <v>1080</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1338,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,14 +1374,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="C3">
         <v>120</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1389,14 +1389,14 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1432,7 +1432,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8">
         <f>SUM(D2:D6)</f>
-        <v>1080</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fonts and image settings
</commit_message>
<xml_diff>
--- a/timing-pie-chart/pie-chart-overview.xlsx
+++ b/timing-pie-chart/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gernotstarke/projects/isaqb/curriculum-foundation/timing-pie-chart/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/curriculum-foundation/timing-pie-chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78513A5B-7F3C-7349-AC2B-E1014585AD85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2CA7FD-ECAE-0241-A8FB-49A75D0A6715}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1180" windowWidth="20700" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="640" windowWidth="20700" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EN-Graphic" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Examples</t>
   </si>
@@ -81,13 +81,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,10 +117,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -133,7 +138,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -162,11 +167,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="5"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-1C48-2F45-B741-7599A94CA97C}"/>
@@ -176,7 +183,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-1C48-2F45-B741-7599A94CA97C}"/>
@@ -186,7 +192,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-1C48-2F45-B741-7599A94CA97C}"/>
@@ -196,7 +201,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-1C48-2F45-B741-7599A94CA97C}"/>
@@ -206,7 +210,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-1C48-2F45-B741-7599A94CA97C}"/>
@@ -216,7 +219,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-1C48-2F45-B741-7599A94CA97C}"/>
@@ -232,8 +234,30 @@
                   <c:y val="-3.3306375106726099E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -253,8 +277,30 @@
                   <c:y val="-3.73477374063182E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -274,8 +320,30 @@
                   <c:y val="6.7844132435252794E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -295,14 +363,54 @@
                   <c:y val="1.8114742434304099E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400">
+                        <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{180DB797-62E6-5D45-8C42-96D0C6E4C223}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US" sz="1400">
+                        <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                        <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      </a:rPr>
+                      <a:pPr>
+                        <a:defRPr sz="1400">
+                          <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                          <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-1C48-2F45-B741-7599A94CA97C}"/>
                 </c:ext>
@@ -316,8 +424,30 @@
                   <c:y val="-5.3475002371691498E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -338,7 +468,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -358,7 +488,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -437,6 +567,9 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -458,7 +591,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -477,11 +610,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="5"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -491,7 +626,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -501,7 +635,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -511,7 +644,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -521,7 +653,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -531,7 +662,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-0D9C-B54A-A4DF-5181D10BBEEC}"/>
@@ -547,8 +677,30 @@
                   <c:y val="-3.3306375106726099E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -568,8 +720,30 @@
                   <c:y val="-3.73477374063182E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -589,8 +763,30 @@
                   <c:y val="6.7844132435252794E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -610,8 +806,30 @@
                   <c:y val="1.8114742434304099E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -631,8 +849,30 @@
                   <c:y val="-5.3475002371691498E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400">
+                      <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                      <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -653,7 +893,7 @@
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
+              <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
@@ -673,7 +913,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -1179,47 +1419,49 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <f>Times!D2</f>
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>Times!D3</f>
         <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f>Times!D4</f>
         <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f>Times!D5</f>
         <v>120</v>
       </c>
@@ -1228,13 +1470,13 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>Times!D6</f>
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="B6" s="1">
         <f>SUM(B1:B5)</f>
         <v>990</v>
       </c>
@@ -1248,80 +1490,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <f>Times!D2</f>
         <v>120</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>Times!D3</f>
         <v>420</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f>Times!D4</f>
         <v>240</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f>Times!D5</f>
         <v>120</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>Times!D6</f>
         <v>90</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
         <f>SUM(B1:B5)</f>
         <v>990</v>
       </c>
@@ -1337,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
+    <sheetView zoomScale="182" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>